<commit_message>
procenti u realne za tezine
</commit_message>
<xml_diff>
--- a/rez.xlsx
+++ b/rez.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aplikacije\parallel-doc-embeds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aplikacije_mihailo\stilometrija\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5F9452-9CCA-4A96-B627-6152AC242226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BFC6D3-E29B-49C2-8942-D94AA2A7F04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B8B4AE92-D4CE-402F-9CE7-E0A30A8665F7}"/>
+    <workbookView xWindow="30000" yWindow="585" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{B8B4AE92-D4CE-402F-9CE7-E0A30A8665F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -302,6 +302,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -445,6 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C12FE24E-7961-459E-B918-F49D7B3E236D}">
   <dimension ref="A2:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A136" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -4722,8 +4726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75CE0FF5-5AD7-4082-85AE-10368F424C96}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="A2:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4750,296 +4754,296 @@
       <c r="A2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="21">
         <v>0.33096417784690801</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="21">
         <v>-0.14706259965896601</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="21">
         <v>0.33025342226028398</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="21">
         <v>0.48584502935409501</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="21">
         <v>0.48835679888725197</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="21">
         <v>6.4648270606994601E-2</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="21">
         <v>0.142275169491767</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="21">
         <v>0.30471986532211298</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="21">
         <v>0.35791182518005299</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="21">
         <v>7.6433934271335602E-2</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="21">
         <v>0.21083749830722801</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="21">
         <v>0.354816764593124</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="21">
         <v>0.21914023160934401</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="21">
         <v>0.201383531093597</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="21">
         <v>4.4196620583534199E-2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="21">
         <v>0.53527963161468495</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="21">
         <v>0.68601405620574896</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="21">
         <v>0.378811925649642</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="21">
         <v>6.3486874103546101E-2</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="21">
         <v>-0.12831278145313199</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="21">
         <v>0.47564777731895402</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="21">
         <v>7.2288393974304199E-2</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="21">
         <v>0.15440456569194699</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="21">
         <v>0.29765921831130898</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="21">
         <v>0.22291065752506201</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="21">
         <v>0.15491573512554099</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="21">
         <v>0.22552852332591999</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="21">
         <v>0.39664506912231401</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="21">
         <v>0.45187640190124501</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="21">
         <v>6.0067467391490902E-2</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="21">
         <v>0.14807434380054399</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="21">
         <v>0.33998182415962203</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="21">
         <v>0.47223582863807601</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="21">
         <v>7.3813647031784002E-2</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="21">
         <v>0.132479533553123</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="21">
         <v>0.32147100567817599</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="21">
         <v>0.40692710876464799</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="21">
         <v>2.8915246948599801E-2</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="21">
         <v>0.210449233651161</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="21">
         <v>0.353708386421203</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="21">
         <v>0.49805065989494302</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="21">
         <v>8.6657613515853799E-2</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="21">
         <v>0.16016976535320199</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="21">
         <v>0.25512203574180597</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="21">
         <v>0.510933697223663</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="21">
         <v>9.7799710929393699E-3</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="21">
         <v>0.17592112720012601</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="21">
         <v>0.30336517095565702</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="21">
         <v>0.418298810720443</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="21">
         <v>-2.3395398631691901E-2</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="21">
         <v>0.182521507143974</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="21">
         <v>0.42257508635520902</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="21">
         <v>0.48616570234298701</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="21">
         <v>7.2063589468598296E-3</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="21">
         <v>0.212303295731544</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="21">
         <v>0.29432466626167297</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="21">
         <v>0.50698661804199197</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="21">
         <v>9.5435403287410694E-2</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="21">
         <v>0.161182790994644</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="21">
         <v>0.23639528453350001</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="21">
         <v>0.38082167506217901</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="21">
         <v>-0.16948443651199299</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="21">
         <v>0.33856853842735202</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="21">
         <v>0.49010974168777399</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="21">
         <v>-4.0015581995248697E-2</v>
       </c>
     </row>
@@ -5047,19 +5051,19 @@
       <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="21">
         <v>0.55756890773773105</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="21">
         <v>2.1341564133763299E-2</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="21">
         <v>7.5580999255180303E-2</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="21">
         <v>0.37339344620704601</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="21">
         <v>-2.78849638998508E-2</v>
       </c>
     </row>
@@ -5067,19 +5071,19 @@
       <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="21">
         <v>0.37253415584564198</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="21">
         <v>0.100581191480159</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="21">
         <v>0.24516396224498699</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="21">
         <v>0.33811503648757901</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="21">
         <v>-5.6394416838884298E-2</v>
       </c>
     </row>
@@ -5087,19 +5091,19 @@
       <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="21">
         <v>0.24280384182929901</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="21">
         <v>0.24130468070507</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="21">
         <v>8.6171969771385096E-2</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="21">
         <v>0.50803250074386597</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="21">
         <v>-7.8312963247299194E-2</v>
       </c>
     </row>
@@ -5107,19 +5111,19 @@
       <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="21">
         <v>0.77561604976653997</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="21">
         <v>0.31022426486015298</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="21">
         <v>7.8258380293846103E-2</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="21">
         <v>-0.11759345978498401</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="21">
         <v>-4.6505283564329099E-2</v>
       </c>
     </row>
@@ -5127,19 +5131,19 @@
       <c r="A23" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="21">
         <v>0.510930776596069</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="21">
         <v>6.7823916673660195E-2</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="21">
         <v>0.15106230974197299</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="21">
         <v>0.31931725144386203</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="21">
         <v>-4.9134299159049898E-2</v>
       </c>
     </row>
@@ -5147,19 +5151,19 @@
       <c r="A24" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="21">
         <v>0.208050176501274</v>
       </c>
-      <c r="C24" s="14">
+      <c r="C24" s="21">
         <v>0.148760005831718</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="21">
         <v>0.225307211279869</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="21">
         <v>0.465918868780136</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="21">
         <v>-4.8036303371190997E-2</v>
       </c>
     </row>
@@ -5167,19 +5171,19 @@
       <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="21">
         <v>0.450052440166473</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="21">
         <v>5.4560143500566399E-2</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="21">
         <v>0.15451422333717299</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="21">
         <v>0.38370195031165999</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="21">
         <v>-4.2828794568777001E-2</v>
       </c>
     </row>
@@ -5187,19 +5191,19 @@
       <c r="A26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="21">
         <v>0.53049874305725098</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="21">
         <v>0.10632412880659101</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="21">
         <v>0.14079058170318601</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="21">
         <v>0.26987919211387601</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="21">
         <v>-4.7492649406194597E-2</v>
       </c>
     </row>
@@ -5207,19 +5211,19 @@
       <c r="A27" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="14">
+      <c r="B27" s="21">
         <v>0.53208369016647294</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="21">
         <v>6.77628293633461E-2</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="21">
         <v>0.17601262032985601</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="21">
         <v>0.27186089754104598</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="21">
         <v>-4.7719944268465E-2</v>
       </c>
     </row>
@@ -5227,19 +5231,19 @@
       <c r="A28" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="21">
         <v>0.501894772052764</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="21">
         <v>7.8864619135856601E-2</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="21">
         <v>0.137695893645286</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="21">
         <v>0.32147237658500599</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="21">
         <v>-3.9927661418914698E-2</v>
       </c>
     </row>
@@ -5247,19 +5251,19 @@
       <c r="A29" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="21">
         <v>0.49523907899856501</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="21">
         <v>2.8192691504955202E-2</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="21">
         <v>0.17762903869152</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="21">
         <v>0.33967560529708801</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="21">
         <v>-4.07363325357437E-2</v>
       </c>
     </row>
@@ -5267,19 +5271,19 @@
       <c r="A30" t="s">
         <v>78</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="21">
         <v>0.37875390052795399</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="21">
         <v>-1.9485631957650101E-2</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="21">
         <v>0.21721754968166301</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="21">
         <v>0.466601401567459</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="21">
         <v>-4.3087188154459E-2</v>
       </c>
     </row>
@@ -5287,19 +5291,19 @@
       <c r="A31" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="21">
         <v>0.40448048710822998</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="21">
         <v>4.5755825936794198E-2</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="21">
         <v>0.19895642995834301</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="21">
         <v>0.39209657907485901</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="21">
         <v>-4.1289363056421197E-2</v>
       </c>
     </row>
@@ -5307,19 +5311,19 @@
       <c r="A32" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="21">
         <v>0.51608401536941495</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="21">
         <v>5.1866505295038202E-2</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="21">
         <v>0.15028204023837999</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="21">
         <v>0.32554730772972101</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="21">
         <v>-4.3779883533716202E-2</v>
       </c>
     </row>
@@ -5381,5 +5385,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>